<commit_message>
Data cleaning and xlsx file
</commit_message>
<xml_diff>
--- a/tables/taco_matching_dict.xlsx
+++ b/tables/taco_matching_dict.xlsx
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>TACO category</t>
+          <t>New category</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>New category</t>
+          <t>Taco category</t>
         </is>
       </c>
     </row>
@@ -451,12 +451,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Metal</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Aerosol</t>
+          <t>Aluminium foil</t>
         </is>
       </c>
     </row>
@@ -466,12 +466,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>E-Waste</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Aluminium blister pack</t>
+          <t>Battery</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Aluminium foil</t>
+          <t>Aluminium blister pack</t>
         </is>
       </c>
     </row>
@@ -496,12 +496,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>E-Waste</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Battery</t>
+          <t>Carded blister pack</t>
         </is>
       </c>
     </row>
@@ -511,12 +511,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Glass</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Broken glass</t>
+          <t>Other plastic bottle</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Carded blister pack</t>
+          <t>Clear plastic bottle</t>
         </is>
       </c>
     </row>
@@ -541,12 +541,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>Glass</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Cigarette</t>
+          <t>Glass bottle</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Clear plastic bottle</t>
+          <t>Plastic bottle cap</t>
         </is>
       </c>
     </row>
@@ -571,12 +571,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Paper</t>
+          <t>Metal</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Corrugated carton</t>
+          <t>Metal bottle cap</t>
         </is>
       </c>
     </row>
@@ -586,12 +586,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Glass</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Crisp packet</t>
+          <t>Broken glass</t>
         </is>
       </c>
     </row>
@@ -601,12 +601,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Disposable food container</t>
+          <t>Food Can</t>
         </is>
       </c>
     </row>
@@ -616,12 +616,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Metal</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Disposable plastic cup</t>
+          <t>Aerosol</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Drink carton</t>
+          <t>Toilet tube</t>
         </is>
       </c>
     </row>
@@ -666,7 +666,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Egg carton</t>
+          <t>Other carton</t>
         </is>
       </c>
     </row>
@@ -676,12 +676,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>Paper</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Foam cup</t>
+          <t>Egg carton</t>
         </is>
       </c>
     </row>
@@ -691,12 +691,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>Paper</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Foam food container</t>
+          <t>Drink carton</t>
         </is>
       </c>
     </row>
@@ -706,12 +706,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>Paper</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Food Can</t>
+          <t>Corrugated carton</t>
         </is>
       </c>
     </row>
@@ -721,12 +721,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Organic</t>
+          <t>Paper</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Food waste</t>
+          <t>Meal carton</t>
         </is>
       </c>
     </row>
@@ -736,12 +736,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>Paper</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Garbage bag</t>
+          <t>Pizza box</t>
         </is>
       </c>
     </row>
@@ -751,12 +751,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Glass</t>
+          <t>Paper</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Glass bottle</t>
+          <t>Paper cup</t>
         </is>
       </c>
     </row>
@@ -766,12 +766,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Glass cup</t>
+          <t>Disposable plastic cup</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Glass</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Glass jar</t>
+          <t>Foam cup</t>
         </is>
       </c>
     </row>
@@ -796,12 +796,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Paper</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Magazine paper</t>
+          <t>Glass cup</t>
         </is>
       </c>
     </row>
@@ -811,12 +811,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Paper</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Meal carton</t>
+          <t>Other plastic cup</t>
         </is>
       </c>
     </row>
@@ -826,12 +826,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Metal</t>
+          <t>Organic</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Metal bottle cap</t>
+          <t>Food waste</t>
         </is>
       </c>
     </row>
@@ -841,12 +841,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Metal</t>
+          <t>Glass</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Metal lid</t>
+          <t>Glass jar</t>
         </is>
       </c>
     </row>
@@ -856,12 +856,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Paper</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Normal paper</t>
+          <t>Plastic lid</t>
         </is>
       </c>
     </row>
@@ -871,12 +871,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Paper</t>
+          <t>Metal</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Other carton</t>
+          <t>Metal lid</t>
         </is>
       </c>
     </row>
@@ -901,12 +901,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Paper</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Other plastic bottle</t>
+          <t>Magazine paper</t>
         </is>
       </c>
     </row>
@@ -916,12 +916,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Other plastic container</t>
+          <t>Tissues</t>
         </is>
       </c>
     </row>
@@ -931,12 +931,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Paper</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Other plastic cup</t>
+          <t>Wrapping paper</t>
         </is>
       </c>
     </row>
@@ -946,12 +946,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Paper</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Other plastic wrapper</t>
+          <t>Normal paper</t>
         </is>
       </c>
     </row>
@@ -961,7 +961,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Paper</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -976,12 +976,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Paper</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Paper cup</t>
+          <t>Plastified paper bag</t>
         </is>
       </c>
     </row>
@@ -991,12 +991,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Paper</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Paper straw</t>
+          <t>Plastic film</t>
         </is>
       </c>
     </row>
@@ -1006,12 +1006,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Paper</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Pizza box</t>
+          <t>Six pack rings</t>
         </is>
       </c>
     </row>
@@ -1021,12 +1021,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Plastic bottle cap</t>
+          <t>Garbage bag</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Plastic film</t>
+          <t>Other plastic wrapper</t>
         </is>
       </c>
     </row>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Plastic glooves</t>
+          <t>Single-use carrier bag</t>
         </is>
       </c>
     </row>
@@ -1066,12 +1066,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Plastic lid</t>
+          <t>Polypropylene bag</t>
         </is>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Plastic straw</t>
+          <t>Crisp packet</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Plastic utensils</t>
+          <t>Spread tub</t>
         </is>
       </c>
     </row>
@@ -1111,12 +1111,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Plastified paper bag</t>
+          <t>Tupperware</t>
         </is>
       </c>
     </row>
@@ -1126,12 +1126,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Polypropylene bag</t>
+          <t>Disposable food container</t>
         </is>
       </c>
     </row>
@@ -1141,12 +1141,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Metal</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Pop tab</t>
+          <t>Foam food container</t>
         </is>
       </c>
     </row>
@@ -1156,12 +1156,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Rope &amp; strings</t>
+          <t>Other plastic container</t>
         </is>
       </c>
     </row>
@@ -1171,12 +1171,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Metal</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Scrap metal</t>
+          <t>Plastic glooves</t>
         </is>
       </c>
     </row>
@@ -1186,12 +1186,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Shoe</t>
+          <t>Plastic utensils</t>
         </is>
       </c>
     </row>
@@ -1201,12 +1201,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Metal</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Single-use carrier bag</t>
+          <t>Pop tab</t>
         </is>
       </c>
     </row>
@@ -1216,12 +1216,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Six pack rings</t>
+          <t>Rope &amp; strings</t>
         </is>
       </c>
     </row>
@@ -1231,12 +1231,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Metal</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Spread tub</t>
+          <t>Scrap metal</t>
         </is>
       </c>
     </row>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Squeezable tube</t>
+          <t>Shoe</t>
         </is>
       </c>
     </row>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Styrofoam piece</t>
+          <t>Squeezable tube</t>
         </is>
       </c>
     </row>
@@ -1276,12 +1276,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Non-recyclable</t>
+          <t>Plastic</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Tissues</t>
+          <t>Plastic straw</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Toilet tube</t>
+          <t>Paper straw</t>
         </is>
       </c>
     </row>
@@ -1306,12 +1306,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Plastic</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Tupperware</t>
+          <t>Styrofoam piece</t>
         </is>
       </c>
     </row>
@@ -1336,12 +1336,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Paper</t>
+          <t>Non-recyclable</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Wrapping paper</t>
+          <t>Cigarette</t>
         </is>
       </c>
     </row>

</xml_diff>